<commit_message>
[IMP] Adjust GL Allowance Doubtful Accounts
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_allowance_doubtful_accounts.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_allowance_doubtful_accounts.xlsx
@@ -59,9 +59,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -147,11 +148,27 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +183,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -252,67 +273,101 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>